<commit_message>
validate+import all employee Excel
</commit_message>
<xml_diff>
--- a/src/WebUI/wwwroot/Ex/employees.xlsx
+++ b/src/WebUI/wwwroot/Ex/employees.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ASP.NET\LogOTAPI\src\WebUI\wwwroot\Ex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rankl\OneDrive\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3420277E-BA9A-4521-A157-0458E0437F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B2DCFD-E353-498F-8AFA-620FB8FABCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B04B188E-7688-4868-AD26-32170FE6FA3D}"/>
   </bookViews>
@@ -36,27 +36,141 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
-  <si>
-    <t>sinh</t>
-  </si>
-  <si>
-    <t>sinh1</t>
-  </si>
-  <si>
-    <t>sinh2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>manager</t>
   </si>
   <si>
     <t>Aa123@</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Trần Công Minh</t>
+  </si>
+  <si>
+    <t>Phùng Xuân Đoan</t>
+  </si>
+  <si>
+    <t>Lưu Thanh Hậu</t>
+  </si>
+  <si>
+    <t>tcm@gmail.com</t>
+  </si>
+  <si>
+    <t>pxd@gmail.com</t>
+  </si>
+  <si>
+    <t>lth@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 Linh Xuân </t>
+  </si>
+  <si>
+    <t>533 Hương Lộ 2</t>
+  </si>
+  <si>
+    <t>344 Gò Dầu</t>
+  </si>
+  <si>
+    <t>minh</t>
+  </si>
+  <si>
+    <t>doan</t>
+  </si>
+  <si>
+    <t>hau</t>
+  </si>
+  <si>
+    <t>0929655358</t>
+  </si>
+  <si>
+    <t>0877654521</t>
+  </si>
+  <si>
+    <t>0777654521</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>19/02/2001</t>
+  </si>
+  <si>
+    <t>17/02/2001</t>
+  </si>
+  <si>
+    <t>20/03/2003</t>
+  </si>
+  <si>
+    <t>VietComBank</t>
+  </si>
+  <si>
+    <t>VietTinBank</t>
+  </si>
+  <si>
+    <t>AgriBank</t>
+  </si>
+  <si>
+    <t>TRANCONGMINH</t>
+  </si>
+  <si>
+    <t>PHUNGXUANDOAN</t>
+  </si>
+  <si>
+    <t>LUUTHANHHAU</t>
+  </si>
+  <si>
+    <t>Tài khoản</t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Hình CCCD</t>
+  </si>
+  <si>
+    <t>Hình đại diện</t>
+  </si>
+  <si>
+    <t>Tên ngân hàng</t>
+  </si>
+  <si>
+    <t>Tên tài khoản</t>
+  </si>
+  <si>
+    <t>tài khoản</t>
+  </si>
+  <si>
+    <t>Mật khẩu</t>
+  </si>
+  <si>
+    <t>Quyền</t>
+  </si>
+  <si>
+    <t>Hình chứng chỉ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="000\-00\-0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,15 +188,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,15 +210,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -414,135 +564,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44526769-E861-4341-BD35-5A143B045FE4}">
-  <dimension ref="A2:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7">
+        <v>2</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="7">
+        <v>123456789</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>123</v>
-      </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="7">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
+      <c r="H3" s="7">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="I3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="7">
+        <v>123456789</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="H4" s="7">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
-        <v>45070.617773692131</v>
-      </c>
-      <c r="G2">
+      <c r="I4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="7">
+        <v>123456789</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>123</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45070.617773692131</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>123</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45070.617773692131</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
+      <c r="N4" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{B87E5DE0-2ECC-4DFD-8A57-599461A6B0CE}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{A994ABCC-D3B7-4382-83F2-D53F0A7FC223}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{35864B66-29D6-4925-8B36-DC4C68D3F858}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{1A820D58-B024-4E3A-9FE0-A58D7D360366}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>